<commit_message>
Added Scrambles for 2025-02-03
</commit_message>
<xml_diff>
--- a/data/2024-12-09/SCW Weekly Comp 2024-12-09 (Responses).xlsx
+++ b/data/2024-12-09/SCW Weekly Comp 2024-12-09 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="215">
   <si>
     <t>Timestamp</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>https://www.facebook.com/events/564322402883911?post_id=572830042033147&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/564322402883911/?post_id=570850372231114&amp;view=permalink&amp;__cft__[0]=AZWYPUbdfgD_GnCoI1UxkN5shTg95VeCBCOYYCGVfebGziPQvIt9VPBjeBEfjl3VsnzuozbshEYQPShpWGG4nC_E6T5cV1Vch5nn47pOC_YcHQPsZXGcJoMlpbJ_LociVh0&amp;__tn__=%2CO%2CP-R</t>
   </si>
 </sst>
 </file>
@@ -836,10 +839,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -847,13 +850,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -982,7 +985,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:DF58" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:DF59" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="110">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -3928,38 +3931,73 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="17">
+      <c r="A58" s="12">
         <v>45648.96660515046</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D58" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E58" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F58" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="CJ58" s="18">
+      <c r="CJ58" s="13">
         <v>45.0</v>
       </c>
-      <c r="CK58" s="18">
+      <c r="CK58" s="13">
         <v>38.0</v>
       </c>
-      <c r="CL58" s="18">
+      <c r="CL58" s="13">
         <v>45.0</v>
       </c>
-      <c r="CM58" s="18">
+      <c r="CM58" s="13">
         <v>38.0</v>
       </c>
-      <c r="CN58" s="18">
+      <c r="CN58" s="13">
         <v>42.67</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="17">
+        <v>45664.05286122685</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="CJ59" s="18">
+        <v>42.0</v>
+      </c>
+      <c r="CK59" s="18">
+        <v>49.0</v>
+      </c>
+      <c r="CL59" s="18">
+        <v>36.0</v>
+      </c>
+      <c r="CM59" s="18">
+        <v>36.0</v>
+      </c>
+      <c r="CN59" s="18">
+        <v>42.33</v>
       </c>
     </row>
   </sheetData>
@@ -4021,10 +4059,11 @@
     <hyperlink r:id="rId55" ref="F56"/>
     <hyperlink r:id="rId56" ref="F57"/>
     <hyperlink r:id="rId57" ref="F58"/>
+    <hyperlink r:id="rId58" ref="F59"/>
   </hyperlinks>
-  <drawing r:id="rId58"/>
+  <drawing r:id="rId59"/>
   <tableParts count="1">
-    <tablePart r:id="rId60"/>
+    <tablePart r:id="rId61"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>